<commit_message>
fixed,and test on sep1
</commit_message>
<xml_diff>
--- a/Prospetto.xlsx
+++ b/Prospetto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\OneDrive\Documenti\GitHub\Tirocinio reelaborated\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4CCAA9-206E-4F6A-B6B0-3C03202D1017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7622820-F012-48A5-9C6A-0DAEC44CB2AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{629C9FE7-9430-448A-85E0-C321F0F6A9B7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>bpic2011_f1</t>
   </si>
@@ -56,24 +56,12 @@
     <t>Tempo</t>
   </si>
   <si>
-    <t>98.70</t>
-  </si>
-  <si>
     <t>Edit Lib</t>
   </si>
   <si>
-    <t>150.5</t>
-  </si>
-  <si>
     <t>Type of encoding</t>
   </si>
   <si>
-    <t>74.39</t>
-  </si>
-  <si>
-    <t>38.58</t>
-  </si>
-  <si>
     <t>weighted_edit 1 1 1</t>
   </si>
   <si>
@@ -137,7 +125,16 @@
     <t>traffic_fines_1</t>
   </si>
   <si>
-    <t>105.38</t>
+    <t>1,39min</t>
+  </si>
+  <si>
+    <t>0,99min</t>
+  </si>
+  <si>
+    <t>0,98min</t>
+  </si>
+  <si>
+    <t>1,00min</t>
   </si>
 </sst>
 </file>
@@ -403,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -427,44 +424,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -473,13 +439,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -488,25 +448,66 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -842,10 +843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA7A6308-527D-488D-8D4E-F071516F402A}">
-  <dimension ref="A1:T22"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -853,681 +854,526 @@
     <col min="1" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="38" t="s">
+    <row r="1" spans="1:17" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="38" t="s">
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="39"/>
-    </row>
-    <row r="2" spans="1:20" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="15" t="s">
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+    </row>
+    <row r="2" spans="1:17" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="26"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="21"/>
       <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="26"/>
+      <c r="G2" s="21"/>
       <c r="H2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="34"/>
+      <c r="I2" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="19"/>
       <c r="K2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" s="34"/>
+      <c r="L2" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="19"/>
       <c r="N2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="P2" s="26"/>
+      <c r="O2" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="21"/>
       <c r="Q2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="R2" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="S2" s="26"/>
-      <c r="T2" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A3" s="13" t="s">
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="10" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="10">
+        <v>0.99</v>
+      </c>
+      <c r="F3" s="31"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="10"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="35"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="25"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="41"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="R3" s="35"/>
-      <c r="S3" s="36"/>
-      <c r="T3" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="20"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="30"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="28"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="15"/>
       <c r="K4" s="6"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="28"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="15"/>
       <c r="N4" s="6"/>
       <c r="O4" s="24"/>
-      <c r="P4" s="23"/>
+      <c r="P4" s="16"/>
       <c r="Q4" s="2"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="4"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="37"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="30"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="28"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="15"/>
       <c r="K5" s="6"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="28"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="15"/>
       <c r="N5" s="6"/>
       <c r="O5" s="24"/>
-      <c r="P5" s="23"/>
+      <c r="P5" s="16"/>
       <c r="Q5" s="2"/>
-      <c r="R5" s="19"/>
-      <c r="S5" s="20"/>
-      <c r="T5" s="4"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="37"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="30"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="28"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="15"/>
       <c r="K6" s="6"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="28"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="15"/>
       <c r="N6" s="6"/>
       <c r="O6" s="24"/>
-      <c r="P6" s="23"/>
+      <c r="P6" s="16"/>
       <c r="Q6" s="2"/>
-      <c r="R6" s="19"/>
-      <c r="S6" s="20"/>
-      <c r="T6" s="4"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="37"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="20"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="30"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="28"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="15"/>
       <c r="K7" s="6"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="28"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="15"/>
       <c r="N7" s="6"/>
       <c r="O7" s="24"/>
-      <c r="P7" s="23"/>
+      <c r="P7" s="16"/>
       <c r="Q7" s="2"/>
-      <c r="R7" s="19"/>
-      <c r="S7" s="20"/>
-      <c r="T7" s="4"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A8" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="37"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="20"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="30"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="28"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="15"/>
       <c r="K8" s="6"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="28"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="15"/>
       <c r="N8" s="6"/>
       <c r="O8" s="24"/>
-      <c r="P8" s="23"/>
+      <c r="P8" s="16"/>
       <c r="Q8" s="2"/>
-      <c r="R8" s="19"/>
-      <c r="S8" s="20"/>
-      <c r="T8" s="4"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A9" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="37"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="20"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="30"/>
       <c r="H9" s="4"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="28"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="15"/>
       <c r="K9" s="6"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="28"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="15"/>
       <c r="N9" s="6"/>
       <c r="O9" s="24"/>
-      <c r="P9" s="23"/>
+      <c r="P9" s="16"/>
       <c r="Q9" s="2"/>
-      <c r="R9" s="19"/>
-      <c r="S9" s="20"/>
-      <c r="T9" s="4"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="37"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="20"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="30"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="28"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="15"/>
       <c r="K10" s="6"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="28"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="15"/>
       <c r="N10" s="6"/>
       <c r="O10" s="24"/>
-      <c r="P10" s="23"/>
+      <c r="P10" s="16"/>
       <c r="Q10" s="2"/>
-      <c r="R10" s="19"/>
-      <c r="S10" s="20"/>
-      <c r="T10" s="4"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="37"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="20"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="30"/>
       <c r="H11" s="4"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="28"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="15"/>
       <c r="K11" s="6"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="28"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="15"/>
       <c r="N11" s="6"/>
       <c r="O11" s="24"/>
-      <c r="P11" s="23"/>
+      <c r="P11" s="16"/>
       <c r="Q11" s="2"/>
-      <c r="R11" s="19"/>
-      <c r="S11" s="20"/>
-      <c r="T11" s="4"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A12" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="37"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="20"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="30"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="28"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="15"/>
       <c r="K12" s="6"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="28"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="15"/>
       <c r="N12" s="6"/>
       <c r="O12" s="24"/>
-      <c r="P12" s="23"/>
+      <c r="P12" s="16"/>
       <c r="Q12" s="2"/>
-      <c r="R12" s="19"/>
-      <c r="S12" s="20"/>
-      <c r="T12" s="4"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="37"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="20"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="30"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="28"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="15"/>
       <c r="K13" s="6"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="28"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="15"/>
       <c r="N13" s="6"/>
       <c r="O13" s="24"/>
-      <c r="P13" s="23"/>
+      <c r="P13" s="16"/>
       <c r="Q13" s="2"/>
-      <c r="R13" s="19"/>
-      <c r="S13" s="20"/>
-      <c r="T13" s="4"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="37"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="20"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="30"/>
       <c r="H14" s="4"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="28"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="15"/>
       <c r="K14" s="6"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="28"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="15"/>
       <c r="N14" s="6"/>
       <c r="O14" s="24"/>
-      <c r="P14" s="23"/>
+      <c r="P14" s="16"/>
       <c r="Q14" s="2"/>
-      <c r="R14" s="19"/>
-      <c r="S14" s="20"/>
-      <c r="T14" s="4"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A15" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="37"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="20"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="30"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="28"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="15"/>
       <c r="K15" s="6"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="28"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="15"/>
       <c r="N15" s="6"/>
       <c r="O15" s="24"/>
-      <c r="P15" s="23"/>
+      <c r="P15" s="16"/>
       <c r="Q15" s="2"/>
-      <c r="R15" s="19"/>
-      <c r="S15" s="20"/>
-      <c r="T15" s="4"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="37"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="20"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="30"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="28"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="15"/>
       <c r="K16" s="6"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="28"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="15"/>
       <c r="N16" s="6"/>
       <c r="O16" s="24"/>
-      <c r="P16" s="23"/>
+      <c r="P16" s="16"/>
       <c r="Q16" s="2"/>
-      <c r="R16" s="19"/>
-      <c r="S16" s="20"/>
-      <c r="T16" s="4"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A17" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A17" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="37"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="20"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="30"/>
       <c r="H17" s="4"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="28"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="15"/>
       <c r="K17" s="6"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="28"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="15"/>
       <c r="N17" s="6"/>
       <c r="O17" s="24"/>
-      <c r="P17" s="23"/>
+      <c r="P17" s="16"/>
       <c r="Q17" s="2"/>
-      <c r="R17" s="19"/>
-      <c r="S17" s="20"/>
-      <c r="T17" s="4"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A18" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A18" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="37"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="20"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="30"/>
       <c r="H18" s="4"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="28"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="15"/>
       <c r="K18" s="6"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="28"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="15"/>
       <c r="N18" s="6"/>
       <c r="O18" s="24"/>
-      <c r="P18" s="23"/>
+      <c r="P18" s="16"/>
       <c r="Q18" s="2"/>
-      <c r="R18" s="19"/>
-      <c r="S18" s="20"/>
-      <c r="T18" s="4"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A19" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="28"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A19" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="37"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="29"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" s="14"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="L19" s="14"/>
+      <c r="M19" s="15"/>
       <c r="N19" s="6"/>
       <c r="O19" s="24"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="19"/>
-      <c r="S19" s="20"/>
-      <c r="T19" s="4"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A20" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="42" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A20" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="37"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="20"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="30"/>
       <c r="H20" s="4"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="28"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="15"/>
       <c r="K20" s="6"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="28"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="15"/>
       <c r="N20" s="6"/>
       <c r="O20" s="24"/>
-      <c r="P20" s="23"/>
+      <c r="P20" s="16"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="19"/>
-      <c r="S20" s="20"/>
-      <c r="T20" s="4"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A21" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A21" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="37"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="20"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="30"/>
       <c r="H21" s="4"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="28"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="15"/>
       <c r="K21" s="6"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="28"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="15"/>
       <c r="N21" s="6"/>
       <c r="O21" s="24"/>
-      <c r="P21" s="23"/>
+      <c r="P21" s="16"/>
       <c r="Q21" s="2"/>
-      <c r="R21" s="19"/>
-      <c r="S21" s="20"/>
-      <c r="T21" s="4"/>
-    </row>
-    <row r="22" spans="1:20" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
+    </row>
+    <row r="22" spans="1:17" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="39"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="22"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="28"/>
       <c r="H22" s="5"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="30"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="26"/>
       <c r="K22" s="7"/>
-      <c r="L22" s="29"/>
-      <c r="M22" s="30"/>
+      <c r="L22" s="25"/>
+      <c r="M22" s="26"/>
       <c r="N22" s="7"/>
-      <c r="O22" s="31"/>
-      <c r="P22" s="32"/>
+      <c r="O22" s="33"/>
+      <c r="P22" s="17"/>
       <c r="Q22" s="3"/>
-      <c r="R22" s="21"/>
-      <c r="S22" s="22"/>
-      <c r="T22" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="150">
-    <mergeCell ref="O1:T1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C1:N1"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="R12:S12"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="R17:S17"/>
-    <mergeCell ref="R18:S18"/>
-    <mergeCell ref="R19:S19"/>
-    <mergeCell ref="R20:S20"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="R10:S10"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
+  <mergeCells count="129">
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="F22:G22"/>
     <mergeCell ref="F16:G16"/>
@@ -1550,27 +1396,91 @@
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C15:D15"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C1:N1"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update to frontend,+override di sicurezza
</commit_message>
<xml_diff>
--- a/Prospetto.xlsx
+++ b/Prospetto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\OneDrive\Documenti\GitHub\Tirocinio reelaborated\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7622820-F012-48A5-9C6A-0DAEC44CB2AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6647350E-E009-4570-AB45-8D72B3F5C283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{629C9FE7-9430-448A-85E0-C321F0F6A9B7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>bpic2011_f1</t>
   </si>
@@ -135,6 +135,18 @@
   </si>
   <si>
     <t>1,00min</t>
+  </si>
+  <si>
+    <t>2,28min</t>
+  </si>
+  <si>
+    <t>1,97min</t>
+  </si>
+  <si>
+    <t>2,71min</t>
+  </si>
+  <si>
+    <t>1,91min</t>
   </si>
 </sst>
 </file>
@@ -424,70 +436,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -505,9 +462,64 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -846,7 +858,7 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -855,503 +867,616 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="11" t="s">
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
     </row>
     <row r="2" spans="1:17" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="21"/>
+      <c r="D2" s="38"/>
       <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="21"/>
+      <c r="G2" s="38"/>
       <c r="H2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="19"/>
+      <c r="J2" s="36"/>
       <c r="K2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="L2" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="19"/>
+      <c r="M2" s="36"/>
       <c r="N2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="20" t="s">
+      <c r="O2" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="21"/>
+      <c r="P2" s="38"/>
       <c r="Q2" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
       <c r="E3" s="10">
         <v>0.99</v>
       </c>
-      <c r="F3" s="31"/>
-      <c r="G3" s="32"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="40"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="21"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="9"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="21"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="38"/>
       <c r="N3" s="9"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="23"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="42"/>
       <c r="Q3" s="10"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="30"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="24"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="15"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="30"/>
       <c r="K4" s="6"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="15"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="30"/>
       <c r="N4" s="6"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="16"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="27"/>
       <c r="Q4" s="2"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="30"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="24"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="15"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="30"/>
       <c r="K5" s="6"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="15"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="30"/>
       <c r="N5" s="6"/>
-      <c r="O5" s="24"/>
-      <c r="P5" s="16"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="27"/>
       <c r="Q5" s="2"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="30"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="24"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="15"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="30"/>
       <c r="K6" s="6"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="15"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="30"/>
       <c r="N6" s="6"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="16"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="27"/>
       <c r="Q6" s="2"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="30"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="24"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="15"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="30"/>
       <c r="K7" s="6"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="15"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="30"/>
       <c r="N7" s="6"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="16"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="27"/>
       <c r="Q7" s="2"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="30"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="24"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="15"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="30"/>
       <c r="K8" s="6"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="15"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="30"/>
       <c r="N8" s="6"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="16"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="27"/>
       <c r="Q8" s="2"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="30"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="24"/>
       <c r="H9" s="4"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="15"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="30"/>
       <c r="K9" s="6"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="15"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="30"/>
       <c r="N9" s="6"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="16"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="27"/>
       <c r="Q9" s="2"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="37"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="30"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="24"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="15"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="30"/>
       <c r="K10" s="6"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="15"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="30"/>
       <c r="N10" s="6"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="16"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="27"/>
       <c r="Q10" s="2"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="30"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="24"/>
       <c r="H11" s="4"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="15"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="30"/>
       <c r="K11" s="6"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="15"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="30"/>
       <c r="N11" s="6"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="16"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="27"/>
       <c r="Q11" s="2"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="30"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="24"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="15"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="30"/>
       <c r="K12" s="6"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="15"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="30"/>
       <c r="N12" s="6"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="16"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="27"/>
       <c r="Q12" s="2"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="30"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="24"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="15"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="30"/>
       <c r="K13" s="6"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="15"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="30"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="16"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="27"/>
       <c r="Q13" s="2"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="30"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="24"/>
       <c r="H14" s="4"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="15"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="30"/>
       <c r="K14" s="6"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="15"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="30"/>
       <c r="N14" s="6"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="16"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="27"/>
       <c r="Q14" s="2"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="30"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="24"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="15"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="30"/>
       <c r="K15" s="6"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="15"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="30"/>
       <c r="N15" s="6"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="16"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="27"/>
       <c r="Q15" s="2"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="30"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="24"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="15"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="30"/>
       <c r="K16" s="6"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="15"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="30"/>
       <c r="N16" s="6"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="16"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="27"/>
       <c r="Q16" s="2"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="30"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="24"/>
       <c r="H17" s="4"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="15"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="30"/>
       <c r="K17" s="6"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="15"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="30"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="16"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="27"/>
       <c r="Q17" s="2"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="30"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="24"/>
       <c r="H18" s="4"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="15"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="30"/>
       <c r="K18" s="6"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="15"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="30"/>
       <c r="N18" s="6"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="16"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="27"/>
       <c r="Q18" s="2"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
       <c r="E19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="29"/>
-      <c r="G19" s="30"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="24"/>
       <c r="H19" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I19" s="14"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="43" t="s">
+      <c r="I19" s="29"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="L19" s="14"/>
-      <c r="M19" s="15"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="30"/>
       <c r="N19" s="6"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="42" t="s">
+      <c r="O19" s="28"/>
+      <c r="P19" s="27"/>
+      <c r="Q19" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="37"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="30"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="24"/>
       <c r="H20" s="4"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="15"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="30"/>
       <c r="K20" s="6"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="15"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="30"/>
       <c r="N20" s="6"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="16"/>
+      <c r="O20" s="28"/>
+      <c r="P20" s="27"/>
       <c r="Q20" s="2"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="37"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="15"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="23"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21" s="29"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L21" s="29"/>
+      <c r="M21" s="30"/>
       <c r="N21" s="6"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="2"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="27"/>
+      <c r="Q21" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="22" spans="1:17" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="28"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="26"/>
       <c r="H22" s="5"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="26"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="32"/>
       <c r="K22" s="7"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="26"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="32"/>
       <c r="N22" s="7"/>
       <c r="O22" s="33"/>
-      <c r="P22" s="17"/>
+      <c r="P22" s="34"/>
       <c r="Q22" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="129">
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C1:N1"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="L14:M14"/>
     <mergeCell ref="O1:Q1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A21:B21"/>
@@ -1376,111 +1501,6 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C1:N1"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>